<commit_message>
add data and graph for Hibernate L1 and L2 cache
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0E82A4-0035-456B-8535-7C726DAC55B3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6948AFC8-2DDD-46E8-914D-8C67E0CB4ACC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>avg</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +54,18 @@
   </si>
   <si>
     <t>mockNum = 1000; mockFollowStep = 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Measuring findAll() in DAO layer in ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeating findAll() in service layer </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeating findAll() in TestUser </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -103,10 +116,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,6 +804,740 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>L1$</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E3FC-4FE3-A72F-20DE796FCD71}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1034536080"/>
+        <c:axId val="1038130688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1034536080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1038130688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1038130688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1034536080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>L2$</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1935</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>945</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>786</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>623</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>593</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>624</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>641</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>597</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>606</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>604</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>592</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>614</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5804-4AE0-92D1-B59020D408EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1130462832"/>
+        <c:axId val="1038264560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1130462832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1038264560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1038264560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1130462832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -871,6 +1618,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1537,6 +2364,1038 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1947,6 +3806,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E801AF4B-5FDD-4FD0-9D93-53F03DB16D58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C54F28AF-CC01-48B4-B2C9-40DF4F8C9F99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98B2BDF8-E892-499C-928B-237CFEA6C9B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2232,7 +4168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -2246,44 +4182,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3">
         <v>1</v>
       </c>
@@ -2302,7 +4238,7 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -2413,42 +4349,42 @@
         <v>1729</v>
       </c>
       <c r="D7" s="1">
-        <f>AVERAGE(D4:D6)</f>
+        <f t="shared" ref="D7:J7" si="1">AVERAGE(D4:D6)</f>
         <v>1840.3333333333333</v>
       </c>
       <c r="E7" s="1">
-        <f>AVERAGE(E4:E6)</f>
+        <f t="shared" si="1"/>
         <v>1566.6666666666667</v>
       </c>
       <c r="F7" s="1">
-        <f>AVERAGE(F4:F6)</f>
+        <f t="shared" si="1"/>
         <v>1474.6666666666667</v>
       </c>
       <c r="G7" s="1">
-        <f>AVERAGE(G4:G6)</f>
+        <f t="shared" si="1"/>
         <v>1330</v>
       </c>
       <c r="H7" s="1">
-        <f>AVERAGE(H4:H6)</f>
+        <f t="shared" si="1"/>
         <v>1337</v>
       </c>
       <c r="I7" s="1">
-        <f>AVERAGE(I4:I6)</f>
+        <f t="shared" si="1"/>
         <v>1177.6666666666667</v>
       </c>
       <c r="J7" s="1">
-        <f>AVERAGE(J4:J6)</f>
+        <f t="shared" si="1"/>
         <v>1126.6666666666667</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="J2:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2458,4 +4394,282 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C8D917-0A82-48FB-A753-E573BC3CB965}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="31.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1736</v>
+      </c>
+      <c r="B3">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>614</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>